<commit_message>
Implementación 001 añadida - NBQ_050100
</commit_message>
<xml_diff>
--- a/ControlCambios/06_Implementacion/Implementacion_001.xlsx
+++ b/ControlCambios/06_Implementacion/Implementacion_001.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/roi_martinez_enriquez_rai_usc_es/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\06_Implementacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{638F9EE2-4F5E-4809-BCD2-CE6D3BF13EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2812DB51-5BB2-4A6B-B649-778BACDE5F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{444F188F-D438-4436-BA11-16438C943C36}"/>
+    <workbookView xWindow="9336" yWindow="0" windowWidth="13800" windowHeight="12336" xr2:uid="{444F188F-D438-4436-BA11-16438C943C36}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementación" sheetId="1" r:id="rId1"/>
@@ -59,93 +59,93 @@
     <t>Nombre:</t>
   </si>
   <si>
-    <t>[Introduzca el nombres completo]</t>
-  </si>
-  <si>
     <t>Correo:</t>
   </si>
   <si>
-    <t>[Introduzca el correo electrónico]</t>
-  </si>
-  <si>
     <t>ID Empleado:</t>
   </si>
   <si>
-    <t>[Número de empleado asignado al gerente]</t>
-  </si>
-  <si>
     <t>Equipo de desarrollo</t>
   </si>
   <si>
     <t>Nombres:</t>
   </si>
   <si>
-    <t>[Introduzca los nombres completos, separados por comas]</t>
-  </si>
-  <si>
     <t>Correos:</t>
   </si>
   <si>
-    <t>[Introduzca los correos en el mismo orden que nombres]</t>
-  </si>
-  <si>
     <t>Cargos:</t>
   </si>
   <si>
-    <t>[Introduzca los cargos, en el mismo orden]</t>
-  </si>
-  <si>
     <t>ID Empleados</t>
   </si>
   <si>
-    <t>[Números de empleados asignados, en el mismo orden]</t>
-  </si>
-  <si>
     <t>Implementación</t>
   </si>
   <si>
     <t>Tiempo real:</t>
   </si>
   <si>
-    <t>[Proporcione el tiempo real de la implementación de los cambios]</t>
-  </si>
-  <si>
     <t>Recursos consumidos:</t>
   </si>
   <si>
-    <t>[Indique los recursos que fueron utilizados durante la implementación ]</t>
-  </si>
-  <si>
     <t>Estado final de los cambios</t>
   </si>
   <si>
-    <t>[Especifíque el resultado final de la implementación de los cambios: /DEFICIENTE/CORRECTA/SOBRESALIENTE]</t>
-  </si>
-  <si>
     <t>Coherencia con la planificación</t>
   </si>
   <si>
-    <t>[Evalue la coherencia entre lo planeado en la planificación y su ejecución: /MÍNIMA/SUSTANCIAL/MODERADA/COMPLETA]</t>
-  </si>
-  <si>
     <t>Incongruencias con la planificación</t>
   </si>
   <si>
-    <t xml:space="preserve">[De existir, indique en qué aspectos se ha producido una planificación deficiente]
+    <t>IMPLEMENTACIÓN</t>
+  </si>
+  <si>
+    <t>1/1</t>
+  </si>
+  <si>
+    <t>Nicolás Barcia Quintela</t>
+  </si>
+  <si>
+    <t>nicolas.barcia@rai.usc.es</t>
+  </si>
+  <si>
+    <t>NBQ_050100</t>
+  </si>
+  <si>
+    <t>Nicolás Barcia Quintela, Jesús Campos Manjón, Guillermo Madriñán González, Roi Martínez Enríquez</t>
+  </si>
+  <si>
+    <t>nicolas.barcia@rai.usc.es, jesus.campos@rai.usc.es, guillermo.madrinan@rai.usc.es, roi.martinez@rai.usc.es</t>
+  </si>
+  <si>
+    <t>Jefe de proyecto, desarrollador, desarrollador, desarrollador</t>
+  </si>
+  <si>
+    <t>NBQ_050100, JCM_180902, GMG_270300, RME_2412002</t>
+  </si>
+  <si>
+    <t>1 semana y 1 día</t>
+  </si>
+  <si>
+    <t>Gerente del proyecto, equipo de desarrollo</t>
+  </si>
+  <si>
+    <t>SOBRESALIENTE</t>
+  </si>
+  <si>
+    <t>MODERADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El proyecto superó el tiempo estimado en un día debido a la necesidad de ajustes en el diseño de la plantilla para grandes volúmenes de datos.
 </t>
-  </si>
-  <si>
-    <t>IMPLEMENTACIÓN</t>
-  </si>
-  <si>
-    <t>1/1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +220,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -777,10 +785,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -794,24 +803,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -826,33 +817,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -860,15 +827,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -880,74 +838,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -960,6 +858,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -972,9 +895,117 @@
     <xf numFmtId="16" fontId="8" fillId="2" borderId="45" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -991,9 +1022,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1031,7 +1062,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1137,7 +1168,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1279,7 +1310,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1290,13 +1321,13 @@
   <dimension ref="C2:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,359 +1345,367 @@
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9" t="s">
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="11" t="s">
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="14"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="15" t="s">
+      <c r="D5" s="51"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="8"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17" t="s">
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17" t="s">
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="15" t="s">
+      <c r="D11" s="61"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="3:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="9"/>
+      <c r="D13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="18" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="3:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="9"/>
+      <c r="D14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="23" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="9"/>
+      <c r="D15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="19"/>
-      <c r="D13" s="20" t="s">
+      <c r="E15" s="15"/>
+      <c r="F15" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="9"/>
+      <c r="D16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="25" t="s">
+      <c r="E16" s="10"/>
+      <c r="F16" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="M17" s="21"/>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C18" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="19"/>
-      <c r="D14" s="20" t="s">
+      <c r="D18" s="51"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C19" s="8"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C20" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="25" t="s">
+      <c r="D20" s="36"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C22" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="30"/>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="19"/>
-      <c r="D15" s="20" t="s">
+      <c r="D22" s="36"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C24" s="9"/>
+      <c r="D24" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="25" t="s">
+      <c r="E24" s="10"/>
+      <c r="F24" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="23"/>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C27" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="30"/>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="19"/>
-      <c r="D16" s="20" t="s">
+      <c r="D27" s="36"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="24"/>
+      <c r="L27" s="25"/>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="7"/>
+      <c r="L28" s="26"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="7"/>
+      <c r="L29" s="26"/>
+    </row>
+    <row r="30" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="31" t="s">
+      <c r="D30" s="41"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="7"/>
+      <c r="L30" s="26"/>
+    </row>
+    <row r="31" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="7"/>
+      <c r="L31" s="26"/>
+    </row>
+    <row r="32" spans="3:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="31"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="33"/>
+      <c r="L32" s="25"/>
+    </row>
+    <row r="33" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34"/>
-    </row>
-    <row r="17" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="37"/>
-      <c r="M17" s="38"/>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="11" t="s">
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C19" s="14"/>
-      <c r="J19" s="13"/>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C20" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="43"/>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="J21" s="13"/>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="13"/>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="19"/>
-      <c r="D24" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="13"/>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="13"/>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="54"/>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="58"/>
-      <c r="L27" s="59"/>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="13"/>
-      <c r="L28" s="60"/>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="13"/>
-      <c r="L29" s="60"/>
-    </row>
-    <row r="30" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="63"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="13"/>
-      <c r="L30" s="60"/>
-    </row>
-    <row r="31" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="65"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="13"/>
-      <c r="L31" s="60"/>
-    </row>
-    <row r="32" spans="3:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="68"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="70"/>
-      <c r="L32" s="59"/>
-    </row>
-    <row r="33" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33" s="74"/>
-    </row>
-    <row r="40" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P40" s="75"/>
+      <c r="J33" s="46"/>
+    </row>
+    <row r="40" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P40" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F24:I25"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:I28"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:I31"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C33:H33"/>
     <mergeCell ref="I33:J33"/>
     <mergeCell ref="F16:I16"/>
@@ -1675,20 +1714,15 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F24:I25"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:I28"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:I31"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{37313EC3-FA8E-4E1F-9758-D8B88CF833E5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Fecha actualizada - NBQ_050100
</commit_message>
<xml_diff>
--- a/ControlCambios/06_Implementacion/Implementacion_001.xlsx
+++ b/ControlCambios/06_Implementacion/Implementacion_001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\06_Implementacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2812DB51-5BB2-4A6B-B649-778BACDE5F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2AD59E-E9FD-43CA-89A6-6D4A5BABE402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9336" yWindow="0" windowWidth="13800" windowHeight="12336" xr2:uid="{444F188F-D438-4436-BA11-16438C943C36}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{444F188F-D438-4436-BA11-16438C943C36}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementación" sheetId="1" r:id="rId1"/>
@@ -859,11 +859,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="2" borderId="44" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="2" borderId="45" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -882,126 +1002,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="2" borderId="44" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="2" borderId="45" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1321,7 +1321,7 @@
   <dimension ref="C2:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1341,29 +1341,29 @@
         <v>2</v>
       </c>
       <c r="I3" s="5">
-        <v>45323</v>
+        <v>45349</v>
       </c>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="67" t="s">
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="68"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="41"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="51"/>
+      <c r="D5" s="43"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -1371,45 +1371,45 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="69" t="s">
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="70" t="s">
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="59" t="s">
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.3">
@@ -1423,10 +1423,10 @@
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="61"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="10"/>
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
@@ -1450,12 +1450,12 @@
         <v>10</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="74" t="s">
+      <c r="F13" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="76"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="53"/>
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="3:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1464,12 +1464,12 @@
         <v>11</v>
       </c>
       <c r="E14" s="15"/>
-      <c r="F14" s="71" t="s">
+      <c r="F14" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="73"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="56"/>
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.3">
@@ -1478,12 +1478,12 @@
         <v>12</v>
       </c>
       <c r="E15" s="15"/>
-      <c r="F15" s="62" t="s">
+      <c r="F15" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="64"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="16"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.3">
@@ -1492,12 +1492,12 @@
         <v>13</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="47" t="s">
+      <c r="F16" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="63"/>
       <c r="J16" s="17"/>
     </row>
     <row r="17" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -1512,10 +1512,10 @@
       <c r="M17" s="21"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="51"/>
+      <c r="D18" s="43"/>
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.3">
@@ -1523,17 +1523,17 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53" t="s">
+      <c r="D20" s="45"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="55"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="67"/>
       <c r="J20" s="22"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.3">
@@ -1543,17 +1543,17 @@
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="56" t="s">
+      <c r="D22" s="45"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="58"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="70"/>
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.3">
@@ -1572,22 +1572,22 @@
         <v>17</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="77" t="s">
+      <c r="F24" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="79"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="73"/>
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="82"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="76"/>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.3">
@@ -1601,17 +1601,17 @@
       <c r="J26" s="23"/>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38" t="s">
+      <c r="D27" s="45"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
       <c r="J27" s="24"/>
       <c r="L27" s="25"/>
     </row>
@@ -1619,10 +1619,10 @@
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
       <c r="J28" s="7"/>
       <c r="L28" s="26"/>
     </row>
@@ -1638,17 +1638,17 @@
       <c r="L29" s="26"/>
     </row>
     <row r="30" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="38" t="s">
+      <c r="D30" s="81"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
       <c r="J30" s="7"/>
       <c r="L30" s="26"/>
     </row>
@@ -1656,10 +1656,10 @@
       <c r="C31" s="28"/>
       <c r="D31" s="29"/>
       <c r="E31" s="30"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
       <c r="J31" s="7"/>
       <c r="L31" s="26"/>
     </row>
@@ -1675,24 +1675,37 @@
       <c r="L32" s="25"/>
     </row>
     <row r="33" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="45" t="s">
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="J33" s="46"/>
+      <c r="J33" s="60"/>
     </row>
     <row r="40" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P40" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F24:I25"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:I28"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:I31"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:J4"/>
@@ -1706,19 +1719,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F24:I25"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:I28"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:I31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{37313EC3-FA8E-4E1F-9758-D8B88CF833E5}"/>

</xml_diff>